<commit_message>
paper stuff and todo
</commit_message>
<xml_diff>
--- a/calculator.xlsx
+++ b/calculator.xlsx
@@ -371,7 +371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
       <selection activeCell="AJ4" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
@@ -500,19 +500,19 @@
         <v>107</v>
       </c>
       <c r="C3">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D3">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E3">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="I3">
         <v>105</v>
@@ -538,15 +538,15 @@
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q11" si="3">C3-J3</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R11" si="4">D3-K3</f>
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S11" si="5">E3-L3</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T11" si="6">F3-M3</f>
@@ -554,11 +554,11 @@
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U11" si="7">G3-N3</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V11" si="8">SUM(ABS(P3)+ABS(Q3) +ABS(R3)+ABS(S3)+ABS(T3)+ABS(U3))/6</f>
-        <v>4.333333333333333</v>
+        <v>8</v>
       </c>
       <c r="W3">
         <v>320</v>
@@ -584,15 +584,15 @@
       </c>
       <c r="AE3" s="1">
         <f t="shared" ref="AE3:AE11" si="10">Q3/X3</f>
-        <v>3.7499999999999999E-2</v>
+        <v>2.8125000000000001E-2</v>
       </c>
       <c r="AF3" s="1">
         <f t="shared" ref="AF3:AF11" si="11">R3/Y3</f>
-        <v>-3.1250000000000002E-3</v>
+        <v>3.125E-2</v>
       </c>
       <c r="AG3" s="1">
         <f t="shared" ref="AG3:AG11" si="12">S3/Z3</f>
-        <v>9.3749999999999997E-3</v>
+        <v>4.3749999999999997E-2</v>
       </c>
       <c r="AH3" s="1">
         <f t="shared" ref="AH3:AH11" si="13">T3/AA3</f>
@@ -600,11 +600,11 @@
       </c>
       <c r="AI3" s="1">
         <f t="shared" ref="AI3:AI11" si="14">U3/AB3</f>
-        <v>3.875968992248062E-2</v>
+        <v>7.7519379844961239E-2</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ11" si="15">SUM(ABS(AD3)+ABS(AE3) +ABS(AF3)+ABS(AG3)+ABS(AH3)+ABS(AI3))/6</f>
-        <v>1.9710917312661499E-2</v>
+        <v>3.5025032299741597E-2</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
@@ -612,22 +612,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D4">
         <v>66</v>
       </c>
       <c r="E4">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G4">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I4">
         <v>135</v>
@@ -649,11 +649,11 @@
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>-17</v>
       </c>
       <c r="Q4">
         <f t="shared" si="3"/>
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="R4">
         <f t="shared" si="4"/>
@@ -661,19 +661,19 @@
       </c>
       <c r="S4">
         <f t="shared" si="5"/>
-        <v>-31</v>
+        <v>-32</v>
       </c>
       <c r="T4">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="U4">
         <f t="shared" si="7"/>
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="V4">
         <f t="shared" si="8"/>
-        <v>17.5</v>
+        <v>17.833333333333332</v>
       </c>
       <c r="W4">
         <v>340</v>
@@ -695,11 +695,11 @@
       </c>
       <c r="AD4" s="1">
         <f t="shared" si="9"/>
-        <v>-4.7058823529411764E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="AE4" s="1">
         <f t="shared" si="10"/>
-        <v>-2.3529411764705882E-2</v>
+        <v>-2.0588235294117647E-2</v>
       </c>
       <c r="AF4" s="1">
         <f t="shared" si="11"/>
@@ -707,19 +707,19 @@
       </c>
       <c r="AG4" s="1">
         <f t="shared" si="12"/>
-        <v>-9.1176470588235289E-2</v>
+        <v>-9.4117647058823528E-2</v>
       </c>
       <c r="AH4" s="1">
         <f t="shared" si="13"/>
-        <v>0.10112359550561797</v>
+        <v>0.11235955056179775</v>
       </c>
       <c r="AI4" s="1">
         <f t="shared" si="14"/>
-        <v>-6.1797752808988762E-2</v>
+        <v>-5.6179775280898875E-2</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="15"/>
-        <v>6.4408460013218774E-2</v>
+        <v>6.5834985679665128E-2</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
@@ -727,22 +727,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C5">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="D5">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E5">
-        <v>270</v>
+        <v>415</v>
       </c>
       <c r="F5">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="I5">
         <v>155</v>
@@ -764,31 +764,31 @@
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>-26</v>
       </c>
       <c r="Q5">
         <f t="shared" si="3"/>
-        <v>-17</v>
+        <v>7</v>
       </c>
       <c r="R5">
         <f t="shared" si="4"/>
-        <v>-24</v>
+        <v>-27</v>
       </c>
       <c r="S5">
         <f t="shared" si="5"/>
-        <v>-39</v>
+        <v>106</v>
       </c>
       <c r="T5">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="U5">
         <f t="shared" si="7"/>
-        <v>-29</v>
+        <v>-12</v>
       </c>
       <c r="V5">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>31.5</v>
       </c>
       <c r="W5">
         <v>440</v>
@@ -810,31 +810,31 @@
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="9"/>
-        <v>4.0909090909090909E-2</v>
+        <v>-5.909090909090909E-2</v>
       </c>
       <c r="AE5" s="1">
         <f t="shared" si="10"/>
-        <v>-3.8636363636363635E-2</v>
+        <v>1.5909090909090907E-2</v>
       </c>
       <c r="AF5" s="1">
         <f t="shared" si="11"/>
-        <v>-5.4545454545454543E-2</v>
+        <v>-6.1363636363636363E-2</v>
       </c>
       <c r="AG5" s="1">
         <f t="shared" si="12"/>
-        <v>-8.8636363636363638E-2</v>
+        <v>0.24090909090909091</v>
       </c>
       <c r="AH5" s="1">
         <f t="shared" si="13"/>
-        <v>9.2391304347826081E-2</v>
+        <v>5.9782608695652176E-2</v>
       </c>
       <c r="AI5" s="1">
         <f t="shared" si="14"/>
-        <v>-0.15760869565217392</v>
+        <v>-6.5217391304347824E-2</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="15"/>
-        <v>7.8787878787878796E-2</v>
+        <v>8.3712121212121196E-2</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
@@ -842,16 +842,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D6">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E6">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -879,19 +879,19 @@
       </c>
       <c r="P6">
         <f t="shared" si="2"/>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="Q6">
         <f t="shared" si="3"/>
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="R6">
         <f t="shared" si="4"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="S6">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T6">
         <f t="shared" si="6"/>
@@ -903,7 +903,7 @@
       </c>
       <c r="V6">
         <f t="shared" si="8"/>
-        <v>17.166666666666668</v>
+        <v>17.333333333333332</v>
       </c>
       <c r="W6">
         <v>270</v>
@@ -925,19 +925,19 @@
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="9"/>
-        <v>-1.4814814814814815E-2</v>
+        <v>-2.2222222222222223E-2</v>
       </c>
       <c r="AE6" s="1">
         <f t="shared" si="10"/>
-        <v>-5.9259259259259262E-2</v>
+        <v>-5.5555555555555552E-2</v>
       </c>
       <c r="AF6" s="1">
         <f t="shared" si="11"/>
-        <v>-5.5555555555555552E-2</v>
+        <v>-4.8148148148148148E-2</v>
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="12"/>
-        <v>0.16296296296296298</v>
+        <v>0.17037037037037037</v>
       </c>
       <c r="AH6" s="1">
         <f t="shared" si="13"/>
@@ -949,7 +949,7 @@
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="15"/>
-        <v>9.272147605480939E-2</v>
+        <v>9.3338760005426666E-2</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
@@ -957,16 +957,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C7">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D7">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E7">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -994,19 +994,19 @@
       </c>
       <c r="P7">
         <f t="shared" si="2"/>
-        <v>-10</v>
+        <v>-1</v>
       </c>
       <c r="Q7">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="R7">
         <f t="shared" si="4"/>
-        <v>-44</v>
+        <v>-27</v>
       </c>
       <c r="S7">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="T7">
         <f t="shared" si="6"/>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="V7">
         <f t="shared" si="8"/>
-        <v>15.166666666666666</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="W7">
         <v>270</v>
@@ -1040,19 +1040,19 @@
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="9"/>
-        <v>-3.7037037037037035E-2</v>
+        <v>-3.7037037037037038E-3</v>
       </c>
       <c r="AE7" s="1">
         <f t="shared" si="10"/>
-        <v>3.7037037037037035E-2</v>
+        <v>-3.7037037037037038E-3</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="11"/>
-        <v>-0.16296296296296298</v>
+        <v>-0.1</v>
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="12"/>
-        <v>3.7037037037037035E-2</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="AH7" s="1">
         <f t="shared" si="13"/>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="15"/>
-        <v>6.9895536562203223E-2</v>
+        <v>5.6932573599240262E-2</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
@@ -1072,22 +1072,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="C8">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="D8">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E8">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I8">
         <v>145</v>
@@ -1109,19 +1109,19 @@
       </c>
       <c r="P8">
         <f t="shared" si="2"/>
-        <v>-17</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="R8">
         <f t="shared" si="4"/>
-        <v>-27</v>
+        <v>-21</v>
       </c>
       <c r="S8">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="T8">
         <f t="shared" si="6"/>
@@ -1129,11 +1129,11 @@
       </c>
       <c r="U8">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="V8">
         <f t="shared" si="8"/>
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="W8">
         <v>386</v>
@@ -1155,19 +1155,19 @@
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="9"/>
-        <v>-4.4041450777202069E-2</v>
+        <v>0</v>
       </c>
       <c r="AE8" s="1">
         <f t="shared" si="10"/>
-        <v>1.8134715025906734E-2</v>
+        <v>-2.3316062176165803E-2</v>
       </c>
       <c r="AF8" s="1">
         <f t="shared" si="11"/>
-        <v>-6.9948186528497408E-2</v>
+        <v>-5.4404145077720206E-2</v>
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="12"/>
-        <v>3.6269430051813469E-2</v>
+        <v>5.6994818652849742E-2</v>
       </c>
       <c r="AH8" s="1">
         <f t="shared" si="13"/>
@@ -1175,11 +1175,11 @@
       </c>
       <c r="AI8" s="1">
         <f t="shared" si="14"/>
-        <v>8.8495575221238937E-2</v>
+        <v>7.0796460176991149E-2</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="15"/>
-        <v>4.2814892934109762E-2</v>
+        <v>3.4251914347287818E-2</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
@@ -1187,22 +1187,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C9">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="D9">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E9">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="I9">
         <v>131</v>
@@ -1224,31 +1224,31 @@
       </c>
       <c r="P9">
         <f t="shared" si="2"/>
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="R9">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="S9">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="U9">
         <f t="shared" si="7"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="V9">
         <f t="shared" si="8"/>
-        <v>7.5</v>
+        <v>3.8333333333333335</v>
       </c>
       <c r="W9">
         <v>386</v>
@@ -1270,31 +1270,31 @@
       </c>
       <c r="AD9" s="1">
         <f t="shared" si="9"/>
-        <v>-1.2953367875647668E-2</v>
+        <v>-2.5906735751295338E-3</v>
       </c>
       <c r="AE9" s="1">
         <f t="shared" si="10"/>
-        <v>-5.1813471502590676E-3</v>
+        <v>2.072538860103627E-2</v>
       </c>
       <c r="AF9" s="1">
         <f t="shared" si="11"/>
-        <v>4.9222797927461141E-2</v>
+        <v>2.8497409326424871E-2</v>
       </c>
       <c r="AG9" s="1">
         <f t="shared" si="12"/>
-        <v>2.072538860103627E-2</v>
+        <v>2.5906735751295338E-3</v>
       </c>
       <c r="AH9" s="1">
         <f t="shared" si="13"/>
-        <v>-2.6666666666666668E-2</v>
+        <v>0</v>
       </c>
       <c r="AI9" s="1">
         <f t="shared" si="14"/>
-        <v>-4.6666666666666669E-2</v>
+        <v>-1.3333333333333334E-2</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="15"/>
-        <v>2.6902705814622913E-2</v>
+        <v>1.128957973517559E-2</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
@@ -1302,16 +1302,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C10">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D10">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1339,19 +1339,19 @@
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="R10">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S10">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="T10">
         <f t="shared" si="6"/>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="V10">
         <f t="shared" si="8"/>
-        <v>5.833333333333333</v>
+        <v>6.5</v>
       </c>
       <c r="W10">
         <v>340</v>
@@ -1385,19 +1385,19 @@
       </c>
       <c r="AD10" s="1">
         <f t="shared" si="9"/>
-        <v>-1.7647058823529412E-2</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="1">
         <f t="shared" si="10"/>
-        <v>5.8823529411764705E-3</v>
+        <v>2.6470588235294117E-2</v>
       </c>
       <c r="AF10" s="1">
         <f t="shared" si="11"/>
-        <v>5.8823529411764705E-3</v>
+        <v>8.8235294117647058E-3</v>
       </c>
       <c r="AG10" s="1">
         <f t="shared" si="12"/>
-        <v>2.3529411764705882E-2</v>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="AH10" s="1">
         <f t="shared" si="13"/>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="AJ10" s="1">
         <f t="shared" si="15"/>
-        <v>3.1490196078431371E-2</v>
+        <v>3.3450980392156861E-2</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
@@ -1417,19 +1417,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C11">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="D11">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E11">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G11">
         <v>132</v>
@@ -1454,23 +1454,23 @@
       </c>
       <c r="P11">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q11">
         <f t="shared" si="3"/>
-        <v>-5</v>
+        <v>20</v>
       </c>
       <c r="R11">
         <f t="shared" si="4"/>
-        <v>-6</v>
+        <v>11</v>
       </c>
       <c r="S11">
         <f t="shared" si="5"/>
-        <v>-18</v>
+        <v>-5</v>
       </c>
       <c r="T11">
         <f t="shared" si="6"/>
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="U11">
         <f t="shared" si="7"/>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="V11">
         <f t="shared" si="8"/>
-        <v>11.166666666666666</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="W11">
         <v>340</v>
@@ -1500,23 +1500,23 @@
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="9"/>
-        <v>3.5294117647058823E-2</v>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="AE11" s="1">
         <f t="shared" si="10"/>
-        <v>-1.4705882352941176E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="AF11" s="1">
         <f t="shared" si="11"/>
-        <v>-1.7647058823529412E-2</v>
+        <v>3.2352941176470591E-2</v>
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="12"/>
-        <v>-5.2941176470588235E-2</v>
+        <v>-1.4705882352941176E-2</v>
       </c>
       <c r="AH11" s="1">
         <f t="shared" si="13"/>
-        <v>-6.25E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="AI11" s="1">
         <f t="shared" si="14"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="AJ11" s="1">
         <f t="shared" si="15"/>
-        <v>4.7181372549019607E-2</v>
+        <v>4.7549019607843135E-2</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">

</xml_diff>